<commit_message>
adding all reply lengths for Timepix
</commit_message>
<xml_diff>
--- a/commands/timepix/timepix_command_deck.xlsx
+++ b/commands/timepix/timepix_command_deck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/timepix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90E2C22-157F-4B46-93B0-7CC9CB3BF306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832BA0A0-D76B-9B41-B9C1-89D4BF0425E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="78">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -256,6 +256,18 @@
   </si>
   <si>
     <t>read something about photon rate</t>
+  </si>
+  <si>
+    <t>0x0c</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x04</t>
   </si>
 </sst>
 </file>
@@ -730,10 +742,10 @@
   <dimension ref="A1:AC19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA11" sqref="AA11:AA19"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1022,9 @@
       <c r="J4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="23"/>
+      <c r="K4" s="23" t="s">
+        <v>74</v>
+      </c>
       <c r="L4" s="6">
         <v>0</v>
       </c>
@@ -1099,7 +1113,9 @@
       <c r="J5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="23"/>
+      <c r="K5" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="L5" s="6">
         <v>0</v>
       </c>
@@ -1188,7 +1204,9 @@
       <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="23" t="s">
+        <v>76</v>
+      </c>
       <c r="L6" s="6">
         <v>0</v>
       </c>
@@ -1277,7 +1295,9 @@
       <c r="J7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="23"/>
+      <c r="K7" s="23" t="s">
+        <v>76</v>
+      </c>
       <c r="L7" s="6">
         <v>0</v>
       </c>
@@ -1366,7 +1386,9 @@
       <c r="J8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="23" t="s">
+        <v>76</v>
+      </c>
       <c r="L8" s="6">
         <v>0</v>
       </c>
@@ -1455,7 +1477,9 @@
       <c r="J9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="23"/>
+      <c r="K9" s="23" t="s">
+        <v>77</v>
+      </c>
       <c r="L9" s="6">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fixed issue: validator.py was omitting first two commands in xlsx sheets.
</commit_message>
<xml_diff>
--- a/commands/timepix/timepix_command_deck.xlsx
+++ b/commands/timepix/timepix_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/timepix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832BA0A0-D76B-9B41-B9C1-89D4BF0425E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA0B8C-3ED6-EA4A-8267-F029DC484328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -745,7 +745,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modifying command codes for timepix to meet jan 15 2024 version of timepix command document
</commit_message>
<xml_diff>
--- a/commands/timepix/timepix_command_deck.xlsx
+++ b/commands/timepix/timepix_command_deck.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/commands/timepix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/timepix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA0B8C-3ED6-EA4A-8267-F029DC484328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F9537D-A47D-E14D-B99B-105490F10525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -258,16 +258,16 @@
     <t>read something about photon rate</t>
   </si>
   <si>
-    <t>0x0c</t>
-  </si>
-  <si>
-    <t>0x03</t>
-  </si>
-  <si>
     <t>0x08</t>
   </si>
   <si>
     <t>0x04</t>
+  </si>
+  <si>
+    <t>0x1b</t>
+  </si>
+  <si>
+    <t>0x09</t>
   </si>
 </sst>
 </file>
@@ -742,10 +742,10 @@
   <dimension ref="A1:AC19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,7 @@
         <v>55</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -1114,7 +1114,7 @@
         <v>32</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>25</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -1264,7 +1264,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="18" t="s">
@@ -1296,7 +1296,7 @@
         <v>59</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -1355,7 +1355,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="18" t="s">
@@ -1387,7 +1387,7 @@
         <v>61</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -1456,11 +1456,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="10">
-        <v>101000</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA8</v>
+        <v>0x81</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
@@ -1478,7 +1478,7 @@
         <v>61</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="AA9" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>0xA8</v>
+        <v>0x81</v>
       </c>
       <c r="AB9" t="s">
         <v>51</v>
@@ -1600,10 +1600,10 @@
         <v>29</v>
       </c>
       <c r="L11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6">
         <v>0</v>
@@ -1612,25 +1612,25 @@
         <v>0</v>
       </c>
       <c r="P11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11" s="16">
         <v>1</v>
@@ -1691,10 +1691,10 @@
         <v>29</v>
       </c>
       <c r="L12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="6">
         <v>0</v>
@@ -1703,25 +1703,25 @@
         <v>0</v>
       </c>
       <c r="P12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="16">
         <v>1</v>
@@ -1757,11 +1757,11 @@
         <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>10001</v>
+        <v>100010</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x11</v>
+        <v>0x22</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>17</v>
@@ -1782,10 +1782,10 @@
         <v>29</v>
       </c>
       <c r="L13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="6">
         <v>0</v>
@@ -1794,25 +1794,25 @@
         <v>0</v>
       </c>
       <c r="P13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13" s="16">
         <v>1</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="AA13" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x11</v>
+        <v>0x22</v>
       </c>
       <c r="AB13" t="s">
         <v>51</v>
@@ -1873,10 +1873,10 @@
         <v>29</v>
       </c>
       <c r="L14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="6">
         <v>0</v>
@@ -1885,25 +1885,25 @@
         <v>0</v>
       </c>
       <c r="P14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" s="16">
         <v>1</v>
@@ -1964,10 +1964,10 @@
         <v>29</v>
       </c>
       <c r="L15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="6">
         <v>0</v>
@@ -1976,25 +1976,25 @@
         <v>0</v>
       </c>
       <c r="P15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15" s="16">
         <v>1</v>
@@ -2055,10 +2055,10 @@
         <v>29</v>
       </c>
       <c r="L16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="6">
         <v>0</v>
@@ -2067,25 +2067,25 @@
         <v>0</v>
       </c>
       <c r="P16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16" s="16">
         <v>1</v>
@@ -2146,10 +2146,10 @@
         <v>29</v>
       </c>
       <c r="L17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" s="6">
         <v>0</v>
@@ -2158,25 +2158,25 @@
         <v>0</v>
       </c>
       <c r="P17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="16">
         <v>1</v>
@@ -2237,10 +2237,10 @@
         <v>29</v>
       </c>
       <c r="L18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="6">
         <v>0</v>
@@ -2249,25 +2249,25 @@
         <v>0</v>
       </c>
       <c r="P18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18" s="16">
         <v>1</v>
@@ -2328,10 +2328,10 @@
         <v>29</v>
       </c>
       <c r="L19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="6">
         <v>0</v>
@@ -2340,25 +2340,25 @@
         <v>0</v>
       </c>
       <c r="P19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" s="16">
         <v>1</v>

</xml_diff>

<commit_message>
adding timepix pcap and event data support. also pushing timepix baud to 115200.
</commit_message>
<xml_diff>
--- a/commands/timepix/timepix_command_deck.xlsx
+++ b/commands/timepix/timepix_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/GSE/GSE-FOXSI-4/foxsi4-commands/commands/timepix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD508E22-E3D1-484E-851F-C9EE4B98A94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE891F0E-AE00-C846-B0AA-A5AD126A7567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="90">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -286,6 +286,24 @@
   </si>
   <si>
     <t>0xff1741</t>
+  </si>
+  <si>
+    <t>read_pcaps</t>
+  </si>
+  <si>
+    <t>read_events</t>
+  </si>
+  <si>
+    <t>events</t>
+  </si>
+  <si>
+    <t>0x5a0</t>
+  </si>
+  <si>
+    <t>read Timepix pcap file summary</t>
+  </si>
+  <si>
+    <t>read photon data for most recent 360 events</t>
   </si>
 </sst>
 </file>
@@ -297,7 +315,7 @@
     <numFmt numFmtId="165" formatCode="00\ 0000\ 00"/>
     <numFmt numFmtId="166" formatCode="0000\ ####"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +362,13 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -389,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -434,6 +459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -443,14 +469,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,13 +784,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AE20"/>
+  <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB14" sqref="AB14:AB20"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -793,51 +812,51 @@
     <col min="25" max="25" width="12.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.1640625" style="20" customWidth="1"/>
     <col min="27" max="27" width="27.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="27.6640625" style="33" customWidth="1"/>
+    <col min="28" max="29" width="27.6640625" style="20" customWidth="1"/>
     <col min="30" max="30" width="19.1640625" customWidth="1"/>
     <col min="31" max="31" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27" t="s">
+      <c r="K1" s="28"/>
+      <c r="L1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="26" t="s">
+      <c r="Y1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -921,10 +940,10 @@
       <c r="AA2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="30" t="s">
+      <c r="AB2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AC2" s="30" t="s">
+      <c r="AC2" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AD2" s="1" t="s">
@@ -948,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E9" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E11" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1018,10 +1037,10 @@
         <f>$E3</f>
         <v>0x80</v>
       </c>
-      <c r="AB3" s="31">
+      <c r="AB3" s="26">
         <v>4</v>
       </c>
-      <c r="AC3" s="34" t="s">
+      <c r="AC3" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD3" t="s">
@@ -1112,13 +1131,13 @@
         <v>29</v>
       </c>
       <c r="AA4" s="25" t="str">
-        <f t="shared" ref="AA4:AA9" si="1">$E4</f>
+        <f t="shared" ref="AA4:AA11" si="1">$E4</f>
         <v>0x88</v>
       </c>
-      <c r="AB4" s="31">
+      <c r="AB4" s="26">
         <v>5</v>
       </c>
-      <c r="AC4" s="34" t="s">
+      <c r="AC4" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD4" t="s">
@@ -1212,10 +1231,10 @@
         <f t="shared" si="1"/>
         <v>0x89</v>
       </c>
-      <c r="AB5" s="31">
+      <c r="AB5" s="26">
         <v>6</v>
       </c>
-      <c r="AC5" s="34" t="s">
+      <c r="AC5" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD5" t="s">
@@ -1309,10 +1328,10 @@
         <f t="shared" si="1"/>
         <v>0x8A</v>
       </c>
-      <c r="AB6" s="31">
+      <c r="AB6" s="26">
         <v>7</v>
       </c>
-      <c r="AC6" s="34" t="s">
+      <c r="AC6" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD6" t="s">
@@ -1406,10 +1425,10 @@
         <f t="shared" si="1"/>
         <v>0x8B</v>
       </c>
-      <c r="AB7" s="31">
+      <c r="AB7" s="26">
         <v>8</v>
       </c>
-      <c r="AC7" s="34" t="s">
+      <c r="AC7" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD7" t="s">
@@ -1503,10 +1522,10 @@
         <f t="shared" si="1"/>
         <v>0xA4</v>
       </c>
-      <c r="AB8" s="31">
+      <c r="AB8" s="26">
         <v>9</v>
       </c>
-      <c r="AC8" s="34" t="s">
+      <c r="AC8" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD8" t="s">
@@ -1517,8 +1536,8 @@
       </c>
     </row>
     <row r="9" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>66</v>
+      <c r="A9" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>41</v>
@@ -1527,11 +1546,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="10">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0x81</v>
+        <v>0xA0</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
@@ -1549,7 +1568,7 @@
         <v>61</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -1598,67 +1617,134 @@
       </c>
       <c r="AA9" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>0x81</v>
-      </c>
-      <c r="AB9" s="31">
+        <v>0xA0</v>
+      </c>
+      <c r="AB9" s="26">
         <v>10</v>
       </c>
-      <c r="AC9" s="34" t="s">
+      <c r="AC9" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD9" t="s">
         <v>51</v>
       </c>
-      <c r="AE9" t="s">
-        <v>73</v>
+      <c r="AE9" s="30" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="32"/>
-      <c r="AC10" s="32"/>
+    <row r="10" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10">
+        <v>100101</v>
+      </c>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>0xA5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+      <c r="R10" s="6">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6">
+        <v>0</v>
+      </c>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="16">
+        <v>1</v>
+      </c>
+      <c r="X10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA10" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>0xA5</v>
+      </c>
+      <c r="AB10" s="26">
+        <v>11</v>
+      </c>
+      <c r="AC10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE10" s="30" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="10">
-        <v>1100010</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f t="shared" ref="E11:E18" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C11,7) + BIN2DEC($D11)))</f>
-        <v>0x62</v>
+        <f t="shared" si="0"/>
+        <v>0x81</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -1673,10 +1759,10 @@
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="K11" s="23" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="L11" s="6">
         <v>0</v>
@@ -1724,122 +1810,55 @@
         <v>29</v>
       </c>
       <c r="AA11" s="25" t="str">
-        <f t="shared" ref="AA11:AA20" si="3">$E11</f>
-        <v>0x62</v>
-      </c>
-      <c r="AB11" s="31">
-        <v>2</v>
-      </c>
-      <c r="AC11" s="34" t="s">
+        <f t="shared" si="1"/>
+        <v>0x81</v>
+      </c>
+      <c r="AB11" s="26">
+        <v>12</v>
+      </c>
+      <c r="AC11" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD11" t="s">
         <v>51</v>
       </c>
       <c r="AE11" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10">
-        <v>1100011</v>
-      </c>
-      <c r="E12" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0x63</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>0</v>
-      </c>
-      <c r="R12" s="6">
-        <v>0</v>
-      </c>
-      <c r="S12" s="6">
-        <v>0</v>
-      </c>
-      <c r="T12" s="6">
-        <v>0</v>
-      </c>
-      <c r="U12" s="6">
-        <v>0</v>
-      </c>
-      <c r="V12" s="6">
-        <v>0</v>
-      </c>
-      <c r="W12" s="16">
-        <v>1</v>
-      </c>
-      <c r="X12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA12" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>0x63</v>
-      </c>
-      <c r="AB12" s="31">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>65</v>
-      </c>
+    <row r="12" spans="1:31" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
     </row>
     <row r="13" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>41</v>
@@ -1848,11 +1867,11 @@
         <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>100010</v>
+        <v>1100010</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0x22</v>
+        <f t="shared" ref="E13:E20" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C13,7) + BIN2DEC($D13)))</f>
+        <v>0x62</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>17</v>
@@ -1918,25 +1937,25 @@
         <v>29</v>
       </c>
       <c r="AA13" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>0x22</v>
-      </c>
-      <c r="AB13" s="31">
-        <v>3</v>
-      </c>
-      <c r="AC13" s="34" t="s">
-        <v>83</v>
+        <f t="shared" ref="AA13:AA22" si="3">$E13</f>
+        <v>0x62</v>
+      </c>
+      <c r="AB13" s="26">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="26" t="s">
+        <v>82</v>
       </c>
       <c r="AD13" t="s">
         <v>51</v>
       </c>
       <c r="AE13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>41</v>
@@ -1945,11 +1964,11 @@
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>1111001</v>
+        <v>1100011</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x79</v>
+        <v>0x63</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -2016,24 +2035,24 @@
       </c>
       <c r="AA14" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x79</v>
-      </c>
-      <c r="AB14" s="31">
-        <v>11</v>
-      </c>
-      <c r="AC14" s="34" t="s">
+        <v>0x63</v>
+      </c>
+      <c r="AB14" s="26">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD14" t="s">
         <v>51</v>
       </c>
       <c r="AE14" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>41</v>
@@ -2042,11 +2061,11 @@
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>1110000</v>
+        <v>100010</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x70</v>
+        <v>0x22</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>17</v>
@@ -2113,24 +2132,24 @@
       </c>
       <c r="AA15" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x70</v>
-      </c>
-      <c r="AB15" s="31">
-        <v>12</v>
-      </c>
-      <c r="AC15" s="34" t="s">
-        <v>82</v>
+        <v>0x22</v>
+      </c>
+      <c r="AB15" s="26">
+        <v>3</v>
+      </c>
+      <c r="AC15" s="26" t="s">
+        <v>83</v>
       </c>
       <c r="AD15" t="s">
         <v>51</v>
       </c>
       <c r="AE15" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>41</v>
@@ -2139,11 +2158,11 @@
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <v>1110001</v>
+        <v>1111001</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x71</v>
+        <v>0x79</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>17</v>
@@ -2210,24 +2229,24 @@
       </c>
       <c r="AA16" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x71</v>
-      </c>
-      <c r="AB16" s="31">
+        <v>0x79</v>
+      </c>
+      <c r="AB16" s="26">
         <v>13</v>
       </c>
-      <c r="AC16" s="34" t="s">
+      <c r="AC16" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD16" t="s">
         <v>51</v>
       </c>
       <c r="AE16" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
+      <c r="A17" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>41</v>
@@ -2236,11 +2255,11 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>1110010</v>
+        <v>1110000</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x72</v>
+        <v>0x70</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>17</v>
@@ -2307,24 +2326,24 @@
       </c>
       <c r="AA17" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x72</v>
-      </c>
-      <c r="AB17" s="31">
+        <v>0x70</v>
+      </c>
+      <c r="AB17" s="26">
         <v>14</v>
       </c>
-      <c r="AC17" s="34" t="s">
+      <c r="AC17" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD17" t="s">
         <v>51</v>
       </c>
       <c r="AE17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>22</v>
+      <c r="A18" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>41</v>
@@ -2333,11 +2352,11 @@
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>1110011</v>
+        <v>1110001</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0x73</v>
+        <v>0x71</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
@@ -2404,24 +2423,24 @@
       </c>
       <c r="AA18" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x73</v>
-      </c>
-      <c r="AB18" s="31">
+        <v>0x71</v>
+      </c>
+      <c r="AB18" s="26">
         <v>15</v>
       </c>
-      <c r="AC18" s="34" t="s">
+      <c r="AC18" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD18" t="s">
         <v>51</v>
       </c>
       <c r="AE18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>41</v>
@@ -2430,11 +2449,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>1110100</v>
+        <v>1110010</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f t="shared" ref="E19:E20" si="4">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C19,7) + BIN2DEC($D19)))</f>
-        <v>0x74</v>
+        <f t="shared" si="2"/>
+        <v>0x72</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -2501,24 +2520,24 @@
       </c>
       <c r="AA19" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>0x74</v>
-      </c>
-      <c r="AB19" s="31">
+        <v>0x72</v>
+      </c>
+      <c r="AB19" s="26">
         <v>16</v>
       </c>
-      <c r="AC19" s="34" t="s">
+      <c r="AC19" s="26" t="s">
         <v>82</v>
       </c>
       <c r="AD19" t="s">
         <v>51</v>
       </c>
       <c r="AE19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>41</v>
@@ -2527,89 +2546,283 @@
         <v>0</v>
       </c>
       <c r="D20" s="10">
+        <v>1110011</v>
+      </c>
+      <c r="E20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0x73</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0</v>
+      </c>
+      <c r="M20" s="6">
+        <v>0</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>0</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0</v>
+      </c>
+      <c r="S20" s="6">
+        <v>0</v>
+      </c>
+      <c r="T20" s="6">
+        <v>0</v>
+      </c>
+      <c r="U20" s="6">
+        <v>0</v>
+      </c>
+      <c r="V20" s="6">
+        <v>0</v>
+      </c>
+      <c r="W20" s="16">
+        <v>1</v>
+      </c>
+      <c r="X20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA20" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>0x73</v>
+      </c>
+      <c r="AB20" s="26">
+        <v>17</v>
+      </c>
+      <c r="AC20" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1110100</v>
+      </c>
+      <c r="E21" s="3" t="str">
+        <f t="shared" ref="E21:E22" si="4">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C21,7) + BIN2DEC($D21)))</f>
+        <v>0x74</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>0</v>
+      </c>
+      <c r="R21" s="6">
+        <v>0</v>
+      </c>
+      <c r="S21" s="6">
+        <v>0</v>
+      </c>
+      <c r="T21" s="6">
+        <v>0</v>
+      </c>
+      <c r="U21" s="6">
+        <v>0</v>
+      </c>
+      <c r="V21" s="6">
+        <v>0</v>
+      </c>
+      <c r="W21" s="16">
+        <v>1</v>
+      </c>
+      <c r="X21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA21" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>0x74</v>
+      </c>
+      <c r="AB21" s="26">
+        <v>18</v>
+      </c>
+      <c r="AC21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
         <v>1111000</v>
       </c>
-      <c r="E20" s="3" t="str">
+      <c r="E22" s="3" t="str">
         <f t="shared" si="4"/>
         <v>0x78</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="6">
-        <v>0</v>
-      </c>
-      <c r="M20" s="6">
-        <v>0</v>
-      </c>
-      <c r="N20" s="6">
-        <v>0</v>
-      </c>
-      <c r="O20" s="6">
-        <v>0</v>
-      </c>
-      <c r="P20" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>0</v>
-      </c>
-      <c r="R20" s="6">
-        <v>0</v>
-      </c>
-      <c r="S20" s="6">
-        <v>0</v>
-      </c>
-      <c r="T20" s="6">
-        <v>0</v>
-      </c>
-      <c r="U20" s="6">
-        <v>0</v>
-      </c>
-      <c r="V20" s="6">
-        <v>0</v>
-      </c>
-      <c r="W20" s="16">
-        <v>1</v>
-      </c>
-      <c r="X20" s="13" t="s">
+      <c r="F22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
+      <c r="R22" s="6">
+        <v>0</v>
+      </c>
+      <c r="S22" s="6">
+        <v>0</v>
+      </c>
+      <c r="T22" s="6">
+        <v>0</v>
+      </c>
+      <c r="U22" s="6">
+        <v>0</v>
+      </c>
+      <c r="V22" s="6">
+        <v>0</v>
+      </c>
+      <c r="W22" s="16">
+        <v>1</v>
+      </c>
+      <c r="X22" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Y20" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA20" s="25" t="str">
+      <c r="Y22" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA22" s="25" t="str">
         <f t="shared" si="3"/>
         <v>0x78</v>
       </c>
-      <c r="AB20" s="31">
-        <v>17</v>
-      </c>
-      <c r="AC20" s="34" t="s">
+      <c r="AB22" s="26">
+        <v>19</v>
+      </c>
+      <c r="AC22" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AD22" t="s">
         <v>51</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AE22" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correcting timepix PC and PCAP request commands, increasing timepix read timeout
</commit_message>
<xml_diff>
--- a/commands/timepix/timepix_command_deck.xlsx
+++ b/commands/timepix/timepix_command_deck.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/GSE/GSE-FOXSI-4/foxsi4-commands/commands/timepix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/timepix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE891F0E-AE00-C846-B0AA-A5AD126A7567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B09BCDE-3EF5-5B48-8ED8-BE4572EF0348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -460,6 +460,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,7 +470,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,7 +790,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -818,43 +818,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
       <c r="X1" s="12"/>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="30"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
@@ -1546,11 +1546,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="10">
-        <v>100000</v>
+        <v>100101</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA0</v>
+        <v>0xA5</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="AA9" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>0xA0</v>
+        <v>0xA5</v>
       </c>
       <c r="AB9" s="26">
         <v>10</v>
@@ -1628,7 +1628,7 @@
       <c r="AD9" t="s">
         <v>51</v>
       </c>
-      <c r="AE9" s="30" t="s">
+      <c r="AE9" s="27" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1643,11 +1643,11 @@
         <v>1</v>
       </c>
       <c r="D10" s="10">
-        <v>100101</v>
+        <v>100000</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>0xA5</v>
+        <v>0xA0</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>17</v>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="AA10" s="25" t="str">
         <f t="shared" si="1"/>
-        <v>0xA5</v>
+        <v>0xA0</v>
       </c>
       <c r="AB10" s="26">
         <v>11</v>
@@ -1725,7 +1725,7 @@
       <c r="AD10" t="s">
         <v>51</v>
       </c>
-      <c r="AE10" s="30" t="s">
+      <c r="AE10" s="27" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>